<commit_message>
initial commit; edited xlsx, added numerator
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -29,13 +29,13 @@
     <t xml:space="preserve">kpi_type</t>
   </si>
   <si>
-    <t xml:space="preserve">entity_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity_3</t>
+    <t xml:space="preserve">filter_entity_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_3</t>
   </si>
   <si>
     <t xml:space="preserve">scene_type</t>
@@ -44,13 +44,13 @@
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
-    <t xml:space="preserve">entity_1_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity_2_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity_3_filter</t>
+    <t xml:space="preserve">filter_entity_1_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_2_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_3_value</t>
   </si>
   <si>
     <t xml:space="preserve">stacking</t>
@@ -74,31 +74,34 @@
     <t xml:space="preserve">MACRO_LINEAR_OWN_MANF_CAT_OUT_OF_STORE</t>
   </si>
   <si>
+    <t xml:space="preserve">manufacturer_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE</t>
+  </si>
+  <si>
     <t xml:space="preserve">manufacturer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub_category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TWE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -137,6 +140,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -186,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,6 +209,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,26 +252,26 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="50.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7295918367347"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.30612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.09183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.52040816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.7295918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="18.3775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,10 +299,10 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -312,94 +325,94 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -414,7 +427,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>19</v>
@@ -471,25 +484,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="41.4795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="40.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="2" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -500,7 +513,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">

</xml_diff>

<commit_message>
added logic to get numerator and denominator and save
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -38,21 +38,21 @@
     <t xml:space="preserve">filter_entity_3</t>
   </si>
   <si>
+    <t xml:space="preserve">filter_entity_1_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_2_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter_entity_3_value</t>
+  </si>
+  <si>
     <t xml:space="preserve">scene_type</t>
   </si>
   <si>
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
-    <t xml:space="preserve">filter_entity_1_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filter_entity_2_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filter_entity_3_value</t>
-  </si>
-  <si>
     <t xml:space="preserve">stacking</t>
   </si>
   <si>
@@ -80,15 +80,12 @@
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
+    <t xml:space="preserve">TWE</t>
+  </si>
+  <si>
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">TWE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White</t>
-  </si>
-  <si>
     <t xml:space="preserve">store</t>
   </si>
   <si>
@@ -101,7 +98,7 @@
     <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE</t>
   </si>
   <si>
-    <t xml:space="preserve">manufacturer</t>
+    <t xml:space="preserve">scene</t>
   </si>
 </sst>
 </file>
@@ -204,18 +201,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,11 +213,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,212 +249,212 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.7397959183674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.7295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.7295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -479,59 +476,59 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="40.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="63.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="19.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing loops, showing calc now
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE</t>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE_TYPE</t>
   </si>
   <si>
     <t xml:space="preserve">scene</t>
@@ -108,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -137,12 +137,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -192,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +207,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,10 +224,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,29 +244,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="1:4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.7397959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.7295918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.9897959183674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,7 +320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -366,8 +365,10 @@
       <c r="P2" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI2" s="6"/>
+      <c r="AMJ2" s="6"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -375,18 +376,14 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="3" t="s">
         <v>20</v>
@@ -412,50 +409,49 @@
       <c r="P3" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="AMI3" s="6"/>
+      <c r="AMJ3" s="6"/>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="0" t="s">
+      <c r="D4" s="3"/>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="O4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="AMI4" s="6"/>
+      <c r="AMJ4" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -476,58 +472,58 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="63.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="19.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="62.3673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor code to make code dry
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zone3_SKU_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zone</t>
   </si>
   <si>
     <t xml:space="preserve">Open Fridge,Fridge Door,Open Impulse Fridge,Standalone Fridge,TWE Open Impulse Fridge,TWE Standalone Fridge</t>
@@ -242,10 +245,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,16 +257,20 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -350,27 +353,27 @@
   <dimension ref="A1:AMH4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P:P"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.6428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.9285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,50 +1575,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P:P A4"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="61.015306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="54.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="15.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="19.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1623,10 +1646,16 @@
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1646,33 +1675,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="1" sqref="P:P L4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="57.6428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="8" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="8" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="9" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.8928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="7" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="18.7704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="11.2602040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1023" min="18" style="7" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="8" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1710,43 +1739,54 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="59.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+    <row r="2" s="9" customFormat="true" ht="70.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="E2" s="10"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="J2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="L2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ2" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
saving twe au custom kpis
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -366,7 +366,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,12 +383,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8B6DE"/>
         <bgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -451,7 +445,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,8 +478,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -500,11 +502,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,15 +534,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,18 +550,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -561,6 +559,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,19 +598,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,11 +622,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -636,7 +634,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -653,7 +655,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -719,30 +721,30 @@
   </sheetPr>
   <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,17 +1948,17 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="50.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="49.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,94 +2047,95 @@
   </sheetPr>
   <dimension ref="1:63"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="8" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="7" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="0"/>
+      <c r="T1" s="10"/>
       <c r="U1" s="0"/>
       <c r="V1" s="0"/>
       <c r="W1" s="0"/>
@@ -3138,2685 +3141,2668 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="13" customFormat="true" ht="71.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    <row r="2" s="15" customFormat="true" ht="71.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="10" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="12"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="15" t="n">
+      <c r="K3" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="L3" s="15" t="n">
+      <c r="L3" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="15" t="s">
+      <c r="M3" s="17"/>
+      <c r="N3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="33.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="15" t="n">
+      <c r="L4" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="15" t="s">
+      <c r="M4" s="17"/>
+      <c r="N4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15" t="s">
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="15" t="s">
+      <c r="S4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="17" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="15" t="n">
+      <c r="L5" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="15" t="s">
+      <c r="M5" s="17"/>
+      <c r="N5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15" t="s">
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="18" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="15" t="n">
+      <c r="K6" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="L6" s="15" t="n">
+      <c r="L6" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="15" t="s">
+      <c r="M6" s="17"/>
+      <c r="N6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15" t="s">
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="15" t="n">
+      <c r="C7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="15" t="s">
+      <c r="M7" s="17"/>
+      <c r="N7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15" t="s">
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S7" s="15" t="s">
+      <c r="S7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="15" t="n">
+      <c r="C8" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="15" t="s">
+      <c r="M8" s="17"/>
+      <c r="N8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15" t="s">
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S8" s="15" t="s">
+      <c r="S8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="15" t="n">
+      <c r="C9" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="15" t="n">
+      <c r="L9" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="15" t="s">
+      <c r="M9" s="17"/>
+      <c r="N9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15" t="s">
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="15" t="s">
+      <c r="R9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S9" s="15" t="s">
+      <c r="S9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="33.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
+      <c r="C10" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20" t="s">
+      <c r="I10" s="21"/>
+      <c r="J10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="20" t="n">
+      <c r="L10" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="20" t="s">
+      <c r="M10" s="21"/>
+      <c r="N10" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20" t="s">
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="20" t="s">
+      <c r="S10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
+      <c r="C11" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20" t="s">
+      <c r="I11" s="21"/>
+      <c r="J11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="20" t="n">
+      <c r="L11" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="20" t="s">
+      <c r="M11" s="21"/>
+      <c r="N11" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20" t="s">
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20" t="s">
+      <c r="C12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="20" t="n">
+      <c r="L12" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" s="20" t="s">
+      <c r="M12" s="21"/>
+      <c r="N12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="Q12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20" t="s">
+      <c r="C13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="21"/>
+      <c r="J13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="20" t="n">
+      <c r="K13" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L13" s="20" t="n">
+      <c r="L13" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="20" t="s">
+      <c r="M13" s="21"/>
+      <c r="N13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20" t="s">
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20" t="s">
+      <c r="C14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20" t="s">
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="L14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" s="20" t="s">
+      <c r="M14" s="21"/>
+      <c r="N14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20" t="s">
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20" t="s">
+      <c r="C15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="20" t="n">
+      <c r="K15" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L15" s="20" t="n">
+      <c r="L15" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O15" s="20" t="s">
+      <c r="M15" s="21"/>
+      <c r="N15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="20" t="s">
+      <c r="P15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q15" s="20" t="s">
+      <c r="Q15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20" t="s">
+      <c r="C16" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L16" s="20" t="s">
+      <c r="L16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" s="20" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="20" t="s">
+      <c r="P16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q16" s="20" t="s">
+      <c r="Q16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R16" s="20" t="s">
+      <c r="R16" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S16" s="20" t="s">
+      <c r="S16" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="23" t="n">
+      <c r="C17" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24" t="s">
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23" t="s">
+      <c r="I17" s="24"/>
+      <c r="J17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="L17" s="23" t="n">
+      <c r="L17" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" s="23" t="s">
+      <c r="M17" s="24"/>
+      <c r="N17" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="23" t="s">
+      <c r="P17" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q17" s="23" t="s">
+      <c r="Q17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="23" t="s">
+      <c r="R17" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S17" s="23" t="s">
+      <c r="S17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="T17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="23" t="n">
+      <c r="C18" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23" t="s">
+      <c r="I18" s="24"/>
+      <c r="J18" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="23" t="n">
+      <c r="K18" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="L18" s="23" t="n">
+      <c r="L18" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O18" s="23" t="s">
+      <c r="M18" s="24"/>
+      <c r="N18" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P18" s="23" t="s">
+      <c r="P18" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q18" s="23" t="s">
+      <c r="Q18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="R18" s="23" t="s">
+      <c r="R18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S18" s="23" t="s">
+      <c r="S18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="T18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="23" t="n">
+      <c r="C19" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24" t="s">
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O19" s="23" t="s">
+      <c r="M19" s="24"/>
+      <c r="N19" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="23" t="s">
+      <c r="P19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q19" s="23" t="s">
+      <c r="Q19" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="R19" s="23" t="s">
+      <c r="R19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S19" s="23" t="s">
+      <c r="S19" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="T19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="74.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="11" t="n">
+      <c r="C20" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="27" t="s">
+      <c r="D20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11" t="s">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" s="11" t="s">
+      <c r="K20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" s="11" t="s">
+      <c r="N20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R20" s="11" t="s">
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="11" t="s">
+      <c r="S20" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="15" t="n">
+      <c r="C21" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15" t="s">
+      <c r="D21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15" t="s">
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="15" t="n">
+      <c r="K21" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="L21" s="15" t="n">
+      <c r="L21" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M21" s="15" t="s">
+      <c r="M21" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" s="15" t="s">
+      <c r="N21" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R21" s="15" t="s">
+      <c r="P21" s="17"/>
+      <c r="Q21" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S21" s="15" t="s">
+      <c r="S21" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15" t="s">
+      <c r="D22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15" t="s">
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="15" t="n">
+      <c r="L22" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="M22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O22" s="15" t="s">
+      <c r="N22" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R22" s="15" t="s">
+      <c r="P22" s="17"/>
+      <c r="Q22" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="15" t="s">
+      <c r="S22" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="15" t="n">
+      <c r="C23" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15" t="s">
+      <c r="D23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15" t="s">
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="15" t="n">
+      <c r="L23" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M23" s="17" t="s">
+      <c r="M23" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N23" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O23" s="15" t="s">
+      <c r="N23" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R23" s="15" t="s">
+      <c r="P23" s="17"/>
+      <c r="Q23" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S23" s="15" t="s">
+      <c r="S23" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="15" t="n">
+      <c r="C24" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15" t="s">
+      <c r="D24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15" t="s">
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="15" t="n">
+      <c r="K24" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="L24" s="15" t="n">
+      <c r="L24" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="N24" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O24" s="15" t="s">
+      <c r="N24" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R24" s="15" t="s">
+      <c r="P24" s="17"/>
+      <c r="Q24" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S24" s="15" t="s">
+      <c r="S24" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15" t="s">
+      <c r="D25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15" t="s">
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="L25" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" s="15" t="s">
+      <c r="N25" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R25" s="15" t="s">
+      <c r="P25" s="17"/>
+      <c r="Q25" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R25" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S25" s="15" t="s">
+      <c r="S25" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="15" t="n">
+      <c r="C26" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15" t="s">
+      <c r="D26" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M26" s="17" t="s">
+      <c r="M26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O26" s="15" t="s">
+      <c r="N26" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R26" s="15" t="s">
+      <c r="P26" s="17"/>
+      <c r="Q26" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S26" s="15" t="s">
+      <c r="S26" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="15" t="n">
+      <c r="C27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15" t="s">
+      <c r="D27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15" t="s">
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="L27" s="15" t="n">
+      <c r="L27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M27" s="17" t="s">
+      <c r="M27" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N27" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O27" s="15" t="s">
+      <c r="N27" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R27" s="15" t="s">
+      <c r="P27" s="17"/>
+      <c r="Q27" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S27" s="15" t="s">
+      <c r="S27" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20" t="s">
+      <c r="C28" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20" t="s">
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="K28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L28" s="20" t="n">
+      <c r="L28" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N28" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" s="20" t="s">
+      <c r="N28" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R28" s="20" t="s">
+      <c r="P28" s="21"/>
+      <c r="Q28" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R28" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S28" s="20" t="s">
+      <c r="S28" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20" t="s">
+      <c r="C29" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20" t="s">
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="20" t="s">
+      <c r="K29" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L29" s="20" t="n">
+      <c r="L29" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="M29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N29" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O29" s="20" t="s">
+      <c r="N29" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R29" s="20" t="s">
+      <c r="P29" s="21"/>
+      <c r="Q29" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R29" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S29" s="20" t="s">
+      <c r="S29" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
+      <c r="C30" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20" t="s">
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="20" t="s">
+      <c r="K30" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="20" t="n">
+      <c r="L30" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M30" s="21" t="s">
+      <c r="M30" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O30" s="20" t="s">
+      <c r="N30" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P30" s="20" t="s">
+      <c r="P30" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q30" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R30" s="20" t="s">
+      <c r="Q30" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R30" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S30" s="20" t="s">
+      <c r="S30" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="63.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20" t="s">
+      <c r="C31" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20" t="s">
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="20" t="n">
+      <c r="K31" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L31" s="20" t="n">
+      <c r="L31" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="M31" s="21" t="s">
+      <c r="M31" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="N31" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O31" s="20" t="s">
+      <c r="N31" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R31" s="20" t="s">
+      <c r="P31" s="21"/>
+      <c r="Q31" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R31" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S31" s="20" t="s">
+      <c r="S31" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20" t="s">
+      <c r="C32" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20" t="s">
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="20" t="s">
+      <c r="K32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L32" s="20" t="s">
+      <c r="L32" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M32" s="20" t="s">
+      <c r="M32" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N32" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O32" s="20" t="s">
+      <c r="N32" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R32" s="20" t="s">
+      <c r="P32" s="21"/>
+      <c r="Q32" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R32" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S32" s="20" t="s">
+      <c r="S32" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20" t="s">
+      <c r="C33" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20" t="s">
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K33" s="20" t="n">
+      <c r="K33" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L33" s="20" t="n">
+      <c r="L33" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N33" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O33" s="20" t="s">
+      <c r="N33" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P33" s="20" t="s">
+      <c r="P33" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q33" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R33" s="20" t="s">
+      <c r="Q33" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R33" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S33" s="20" t="s">
+      <c r="S33" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20" t="s">
+      <c r="C34" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20" t="s">
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K34" s="20" t="s">
+      <c r="K34" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L34" s="20" t="s">
+      <c r="L34" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M34" s="21" t="s">
+      <c r="M34" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N34" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O34" s="20" t="s">
+      <c r="N34" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P34" s="20" t="s">
+      <c r="P34" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q34" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R34" s="20" t="s">
+      <c r="Q34" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R34" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S34" s="20" t="s">
+      <c r="S34" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="23" t="n">
+      <c r="C35" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D35" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23" t="s">
+      <c r="D35" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H35" s="24"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23" t="s">
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K35" s="23" t="s">
+      <c r="K35" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="L35" s="23" t="n">
+      <c r="L35" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="M35" s="24" t="s">
+      <c r="M35" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O35" s="23" t="s">
+      <c r="N35" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P35" s="23" t="s">
+      <c r="P35" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q35" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R35" s="23" t="s">
+      <c r="Q35" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R35" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S35" s="23" t="s">
+      <c r="S35" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="23" t="n">
+      <c r="C36" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23" t="s">
+      <c r="D36" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="24"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23" t="s">
+      <c r="H36" s="25"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K36" s="23" t="s">
+      <c r="K36" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L36" s="23" t="s">
+      <c r="L36" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M36" s="24" t="s">
+      <c r="M36" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="N36" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O36" s="23" t="s">
+      <c r="N36" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P36" s="23" t="s">
+      <c r="P36" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q36" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R36" s="23" t="s">
+      <c r="Q36" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R36" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S36" s="23" t="s">
+      <c r="S36" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="23" t="n">
+      <c r="C37" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23" t="s">
+      <c r="D37" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23" t="s">
+      <c r="H37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K37" s="23" t="n">
+      <c r="K37" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="L37" s="23" t="n">
+      <c r="L37" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="M37" s="24" t="s">
+      <c r="M37" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="N37" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O37" s="23" t="s">
+      <c r="N37" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P37" s="23" t="s">
+      <c r="P37" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q37" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R37" s="23" t="s">
+      <c r="Q37" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R37" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S37" s="23" t="s">
+      <c r="S37" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="83.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="11" t="n">
+      <c r="C38" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="27" t="s">
+      <c r="F38" s="13"/>
+      <c r="G38" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11" t="s">
+      <c r="I38" s="13"/>
+      <c r="J38" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L38" s="11" t="s">
+      <c r="K38" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O38" s="11" t="s">
+      <c r="M38" s="13"/>
+      <c r="N38" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R38" s="11" t="s">
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="R38" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="S38" s="11" t="s">
+      <c r="S38" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="46.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="15" t="n">
+      <c r="C39" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="15" t="s">
+      <c r="D39" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15" t="s">
+      <c r="F39" s="17"/>
+      <c r="G39" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H39" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15" t="s">
+      <c r="I39" s="17"/>
+      <c r="J39" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="K39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="L39" s="15" t="n">
+      <c r="L39" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O39" s="15" t="s">
+      <c r="M39" s="17"/>
+      <c r="N39" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R39" s="15" t="s">
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R39" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S39" s="15" t="s">
+      <c r="S39" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="15" t="n">
+      <c r="C40" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D40" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="15" t="s">
+      <c r="D40" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15" t="s">
+      <c r="F40" s="17"/>
+      <c r="G40" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15" t="s">
+      <c r="I40" s="17"/>
+      <c r="J40" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="15" t="s">
+      <c r="K40" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L40" s="15" t="s">
+      <c r="L40" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O40" s="15" t="s">
+      <c r="M40" s="17"/>
+      <c r="N40" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R40" s="15" t="s">
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R40" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S40" s="15" t="s">
+      <c r="S40" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="15" t="n">
+      <c r="C41" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="15" t="s">
+      <c r="D41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15" t="s">
+      <c r="F41" s="17"/>
+      <c r="G41" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15" t="s">
+      <c r="I41" s="17"/>
+      <c r="J41" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L41" s="15" t="s">
+      <c r="L41" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O41" s="15" t="s">
+      <c r="M41" s="17"/>
+      <c r="N41" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R41" s="15" t="s">
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R41" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S41" s="15" t="s">
+      <c r="S41" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="15" t="n">
+      <c r="C42" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="15" t="s">
+      <c r="D42" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15" t="s">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15" t="s">
+      <c r="I42" s="17"/>
+      <c r="J42" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K42" s="15" t="n">
+      <c r="K42" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="L42" s="15" t="n">
+      <c r="L42" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O42" s="15" t="s">
+      <c r="M42" s="17"/>
+      <c r="N42" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R42" s="15" t="s">
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R42" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S42" s="15" t="s">
+      <c r="S42" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="15" t="n">
+      <c r="C43" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="15" t="s">
+      <c r="D43" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15" t="s">
+      <c r="F43" s="17"/>
+      <c r="G43" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15" t="s">
+      <c r="I43" s="17"/>
+      <c r="J43" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L43" s="15" t="n">
+      <c r="L43" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O43" s="15" t="s">
+      <c r="M43" s="17"/>
+      <c r="N43" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R43" s="15" t="s">
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R43" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S43" s="15" t="s">
+      <c r="S43" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="53.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="15" t="n">
+      <c r="C44" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="15" t="s">
+      <c r="D44" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15" t="s">
+      <c r="F44" s="17"/>
+      <c r="G44" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15" t="s">
+      <c r="I44" s="17"/>
+      <c r="J44" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="K44" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L44" s="15" t="n">
+      <c r="L44" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O44" s="15" t="s">
+      <c r="M44" s="17"/>
+      <c r="N44" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R44" s="15" t="s">
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R44" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S44" s="15" t="s">
+      <c r="S44" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="15" t="n">
+      <c r="C45" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="15" t="s">
+      <c r="D45" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15" t="s">
+      <c r="F45" s="17"/>
+      <c r="G45" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15" t="s">
+      <c r="I45" s="17"/>
+      <c r="J45" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K45" s="15" t="n">
+      <c r="K45" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="L45" s="15" t="n">
+      <c r="L45" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O45" s="15" t="s">
+      <c r="M45" s="17"/>
+      <c r="N45" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O45" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R45" s="15" t="s">
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R45" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S45" s="15" t="s">
+      <c r="S45" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="20" t="s">
+      <c r="C46" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20" t="s">
+      <c r="F46" s="21"/>
+      <c r="G46" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20" t="s">
+      <c r="I46" s="21"/>
+      <c r="J46" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K46" s="20" t="s">
+      <c r="K46" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L46" s="20" t="n">
+      <c r="L46" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O46" s="20" t="s">
+      <c r="M46" s="21"/>
+      <c r="N46" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R46" s="20" t="s">
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R46" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S46" s="20" t="s">
+      <c r="S46" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="20" t="s">
+      <c r="C47" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20" t="s">
+      <c r="F47" s="21"/>
+      <c r="G47" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20" t="s">
+      <c r="I47" s="21"/>
+      <c r="J47" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K47" s="20" t="s">
+      <c r="K47" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L47" s="20" t="n">
+      <c r="L47" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O47" s="20" t="s">
+      <c r="M47" s="21"/>
+      <c r="N47" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R47" s="20" t="s">
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R47" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S47" s="20" t="s">
+      <c r="S47" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="55.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="20" t="s">
+      <c r="C48" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20" t="s">
+      <c r="F48" s="21"/>
+      <c r="G48" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20" t="s">
+      <c r="I48" s="21"/>
+      <c r="J48" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K48" s="20" t="s">
+      <c r="K48" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L48" s="20" t="n">
+      <c r="L48" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="M48" s="20"/>
-      <c r="N48" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O48" s="20" t="s">
+      <c r="M48" s="21"/>
+      <c r="N48" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P48" s="20" t="s">
+      <c r="P48" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q48" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R48" s="20" t="s">
+      <c r="Q48" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R48" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S48" s="20" t="s">
+      <c r="S48" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="20" t="s">
+      <c r="C49" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20" t="s">
+      <c r="F49" s="21"/>
+      <c r="G49" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="H49" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="I49" s="37"/>
-      <c r="J49" s="20" t="s">
+      <c r="I49" s="38"/>
+      <c r="J49" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K49" s="20" t="n">
+      <c r="K49" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L49" s="20" t="n">
+      <c r="L49" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="M49" s="20"/>
-      <c r="N49" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O49" s="20" t="s">
+      <c r="M49" s="21"/>
+      <c r="N49" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="P49" s="20"/>
-      <c r="Q49" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R49" s="20" t="s">
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R49" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S49" s="20" t="s">
+      <c r="S49" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="20" t="s">
+      <c r="C50" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20" t="s">
+      <c r="F50" s="21"/>
+      <c r="G50" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H50" s="37" t="s">
+      <c r="H50" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="I50" s="37"/>
-      <c r="J50" s="20" t="s">
+      <c r="I50" s="38"/>
+      <c r="J50" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K50" s="20" t="s">
+      <c r="K50" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L50" s="20" t="s">
+      <c r="L50" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R50" s="20" t="s">
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R50" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S50" s="20"/>
+      <c r="S50" s="21"/>
     </row>
     <row r="51" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="20" t="s">
+      <c r="C51" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20" t="s">
+      <c r="F51" s="21"/>
+      <c r="G51" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H51" s="37" t="s">
+      <c r="H51" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I51" s="37"/>
-      <c r="J51" s="20" t="s">
+      <c r="I51" s="38"/>
+      <c r="J51" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K51" s="20" t="n">
+      <c r="K51" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="L51" s="20" t="n">
+      <c r="L51" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20" t="s">
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q51" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R51" s="20" t="s">
+      <c r="Q51" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R51" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S51" s="20"/>
+      <c r="S51" s="21"/>
     </row>
     <row r="52" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="20" t="s">
+      <c r="C52" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20" t="s">
+      <c r="F52" s="21"/>
+      <c r="G52" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H52" s="37" t="s">
+      <c r="H52" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I52" s="37"/>
-      <c r="J52" s="20" t="s">
+      <c r="I52" s="38"/>
+      <c r="J52" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K52" s="20" t="s">
+      <c r="K52" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L52" s="20" t="s">
+      <c r="L52" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20" t="s">
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q52" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R52" s="20" t="s">
+      <c r="Q52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S52" s="20"/>
+      <c r="S52" s="21"/>
     </row>
     <row r="53" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="23" t="n">
+      <c r="C53" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D53" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="23" t="s">
+      <c r="D53" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23" t="s">
+      <c r="F53" s="24"/>
+      <c r="G53" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H53" s="24" t="s">
+      <c r="H53" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23" t="s">
+      <c r="I53" s="24"/>
+      <c r="J53" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K53" s="23" t="s">
+      <c r="K53" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="L53" s="23" t="n">
+      <c r="L53" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="M53" s="23"/>
-      <c r="N53" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O53" s="23" t="s">
+      <c r="M53" s="24"/>
+      <c r="N53" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P53" s="23" t="s">
+      <c r="P53" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q53" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R53" s="23" t="s">
+      <c r="Q53" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R53" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="S53" s="23" t="s">
+      <c r="S53" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="23" t="n">
+      <c r="C54" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D54" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="23" t="s">
+      <c r="D54" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23" t="s">
+      <c r="F54" s="24"/>
+      <c r="G54" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H54" s="24" t="s">
+      <c r="H54" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23" t="s">
+      <c r="I54" s="24"/>
+      <c r="J54" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K54" s="23" t="n">
+      <c r="K54" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="L54" s="23" t="n">
+      <c r="L54" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="M54" s="23"/>
-      <c r="N54" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O54" s="23" t="s">
+      <c r="M54" s="24"/>
+      <c r="N54" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P54" s="23" t="s">
+      <c r="P54" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q54" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R54" s="23" t="s">
+      <c r="Q54" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R54" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="S54" s="23" t="s">
+      <c r="S54" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="23" t="n">
+      <c r="C55" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D55" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="23" t="s">
+      <c r="D55" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23" t="s">
+      <c r="F55" s="24"/>
+      <c r="G55" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23" t="s">
+      <c r="I55" s="24"/>
+      <c r="J55" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="23" t="s">
+      <c r="K55" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L55" s="23" t="s">
+      <c r="L55" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M55" s="23"/>
-      <c r="N55" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O55" s="23" t="s">
+      <c r="M55" s="24"/>
+      <c r="N55" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O55" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="P55" s="23" t="s">
+      <c r="P55" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Q55" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="R55" s="23" t="s">
+      <c r="Q55" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="R55" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="S55" s="23" t="s">
+      <c r="S55" s="24" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5846,159 +5832,159 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="38" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="38" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="38" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="38" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="38" width="54.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="38" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="39" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="39" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="E2" s="43"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42" t="s">
+      <c r="B3" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="E3" s="43"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="E4" s="43"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42" t="s">
+      <c r="B5" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="E5" s="43"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="42" t="s">
+      <c r="B6" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="G6" s="44"/>
+      <c r="E6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="42" t="s">
+      <c r="B7" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="45"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="42" t="s">
+      <c r="B8" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="45"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="42" t="s">
+      <c r="B9" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="45"/>
+      <c r="E9" s="46"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixing manufacturer name in linear kpi
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Linear KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="65">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
-    <t xml:space="preserve">TWE</t>
+    <t xml:space="preserve">Treasury Wine Estates</t>
   </si>
   <si>
     <t xml:space="preserve">All</t>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t xml:space="preserve">ZONE3_OWN_MANUFACTURER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treasury Wine Estates</t>
   </si>
   <si>
     <t xml:space="preserve">Open Fridge,
@@ -721,8 +718,8 @@
   </sheetPr>
   <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1948,8 +1945,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2047,10 +2044,10 @@
   </sheetPr>
   <dimension ref="1:63"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4016,7 +4013,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="28" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -4030,7 +4027,7 @@
         <v>34</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N20" s="13" t="n">
         <v>1</v>
@@ -4051,10 +4048,10 @@
     </row>
     <row r="21" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>4</v>
@@ -4065,7 +4062,7 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
@@ -4100,10 +4097,10 @@
     </row>
     <row r="22" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>4</v>
@@ -4114,7 +4111,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
@@ -4149,10 +4146,10 @@
     </row>
     <row r="23" customFormat="false" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="17" t="n">
         <v>4</v>
@@ -4163,7 +4160,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -4198,10 +4195,10 @@
     </row>
     <row r="24" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="17" t="n">
         <v>4</v>
@@ -4212,7 +4209,7 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -4226,7 +4223,7 @@
         <v>3</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N24" s="17" t="n">
         <v>1</v>
@@ -4247,10 +4244,10 @@
     </row>
     <row r="25" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="17" t="n">
         <v>4</v>
@@ -4261,7 +4258,7 @@
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -4296,10 +4293,10 @@
     </row>
     <row r="26" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="17" t="n">
         <v>4</v>
@@ -4310,7 +4307,7 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
@@ -4345,10 +4342,10 @@
     </row>
     <row r="27" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="17" t="n">
         <v>4</v>
@@ -4359,7 +4356,7 @@
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
@@ -4394,10 +4391,10 @@
     </row>
     <row r="28" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="21" t="n">
         <v>1</v>
@@ -4408,7 +4405,7 @@
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -4443,10 +4440,10 @@
     </row>
     <row r="29" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="21" t="n">
         <v>1</v>
@@ -4457,7 +4454,7 @@
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
@@ -4492,10 +4489,10 @@
     </row>
     <row r="30" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="21" t="n">
         <v>1</v>
@@ -4506,7 +4503,7 @@
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
@@ -4543,10 +4540,10 @@
     </row>
     <row r="31" customFormat="false" ht="63.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="21" t="n">
         <v>1</v>
@@ -4557,7 +4554,7 @@
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
@@ -4592,10 +4589,10 @@
     </row>
     <row r="32" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="21" t="n">
         <v>1</v>
@@ -4606,7 +4603,7 @@
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
       <c r="G32" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
@@ -4641,10 +4638,10 @@
     </row>
     <row r="33" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="21" t="n">
         <v>1</v>
@@ -4655,7 +4652,7 @@
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
@@ -4692,10 +4689,10 @@
     </row>
     <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="21" t="n">
         <v>1</v>
@@ -4706,7 +4703,7 @@
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
@@ -4743,10 +4740,10 @@
     </row>
     <row r="35" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="24" t="n">
         <v>2</v>
@@ -4757,7 +4754,7 @@
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="24"/>
@@ -4794,10 +4791,10 @@
     </row>
     <row r="36" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="24" t="n">
         <v>2</v>
@@ -4808,7 +4805,7 @@
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
       <c r="G36" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H36" s="25"/>
       <c r="I36" s="24"/>
@@ -4845,10 +4842,10 @@
     </row>
     <row r="37" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="24" t="n">
         <v>2</v>
@@ -4859,7 +4856,7 @@
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
       <c r="G37" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H37" s="25"/>
       <c r="I37" s="24"/>
@@ -4896,10 +4893,10 @@
     </row>
     <row r="38" customFormat="false" ht="83.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="13" t="n">
         <v>3</v>
@@ -4912,10 +4909,10 @@
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13" t="s">
@@ -4947,10 +4944,10 @@
     </row>
     <row r="39" customFormat="false" ht="46.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>4</v>
@@ -4963,7 +4960,7 @@
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H39" s="18" t="s">
         <v>41</v>
@@ -4998,10 +4995,10 @@
     </row>
     <row r="40" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>4</v>
@@ -5014,7 +5011,7 @@
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>39</v>
@@ -5049,10 +5046,10 @@
     </row>
     <row r="41" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="17" t="n">
         <v>4</v>
@@ -5065,7 +5062,7 @@
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>41</v>
@@ -5100,10 +5097,10 @@
     </row>
     <row r="42" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="17" t="n">
         <v>4</v>
@@ -5116,7 +5113,7 @@
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>39</v>
@@ -5151,10 +5148,10 @@
     </row>
     <row r="43" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="17" t="n">
         <v>4</v>
@@ -5167,7 +5164,7 @@
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>39</v>
@@ -5202,10 +5199,10 @@
     </row>
     <row r="44" customFormat="false" ht="53.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="17" t="n">
         <v>4</v>
@@ -5218,7 +5215,7 @@
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>41</v>
@@ -5253,10 +5250,10 @@
     </row>
     <row r="45" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" s="17" t="n">
         <v>4</v>
@@ -5269,10 +5266,10 @@
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="17" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="17" t="s">
@@ -5304,10 +5301,10 @@
     </row>
     <row r="46" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="21" t="n">
         <v>1</v>
@@ -5320,7 +5317,7 @@
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>39</v>
@@ -5355,10 +5352,10 @@
     </row>
     <row r="47" customFormat="false" ht="21.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" s="21" t="n">
         <v>1</v>
@@ -5371,7 +5368,7 @@
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H47" s="21" t="s">
         <v>39</v>
@@ -5406,10 +5403,10 @@
     </row>
     <row r="48" customFormat="false" ht="55.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="21" t="n">
         <v>1</v>
@@ -5422,7 +5419,7 @@
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H48" s="22" t="s">
         <v>41</v>
@@ -5459,10 +5456,10 @@
     </row>
     <row r="49" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="21" t="n">
         <v>1</v>
@@ -5475,10 +5472,10 @@
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H49" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I49" s="38"/>
       <c r="J49" s="21" t="s">
@@ -5510,10 +5507,10 @@
     </row>
     <row r="50" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="21" t="n">
         <v>1</v>
@@ -5526,7 +5523,7 @@
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H50" s="38" t="s">
         <v>39</v>
@@ -5555,10 +5552,10 @@
     </row>
     <row r="51" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="21" t="n">
         <v>1</v>
@@ -5571,7 +5568,7 @@
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H51" s="38" t="s">
         <v>41</v>
@@ -5602,10 +5599,10 @@
     </row>
     <row r="52" customFormat="false" ht="36.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="21" t="n">
         <v>1</v>
@@ -5618,7 +5615,7 @@
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="21" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H52" s="38" t="s">
         <v>41</v>
@@ -5649,10 +5646,10 @@
     </row>
     <row r="53" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="24" t="n">
         <v>2</v>
@@ -5665,7 +5662,7 @@
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H53" s="25" t="s">
         <v>41</v>
@@ -5702,10 +5699,10 @@
     </row>
     <row r="54" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="24" t="n">
         <v>2</v>
@@ -5718,7 +5715,7 @@
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H54" s="25" t="s">
         <v>41</v>
@@ -5755,10 +5752,10 @@
     </row>
     <row r="55" customFormat="false" ht="49.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="24" t="n">
         <v>2</v>
@@ -5771,7 +5768,7 @@
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="24" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H55" s="25" t="s">
         <v>41</v>
@@ -5832,7 +5829,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -5878,7 +5875,7 @@
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E2" s="43"/>
       <c r="G2" s="41"/>
@@ -5887,14 +5884,14 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E3" s="43"/>
       <c r="G3" s="41"/>
@@ -5903,14 +5900,14 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E4" s="43"/>
       <c r="G4" s="41"/>
@@ -5919,14 +5916,14 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E5" s="43"/>
       <c r="G5" s="41"/>
@@ -5935,54 +5932,54 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E6" s="46"/>
       <c r="G6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="43" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E9" s="46"/>
     </row>

</xml_diff>

<commit_message>
fixing bugs with calculations where no products were present
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -635,30 +635,30 @@
   <dimension ref="A1:AMI4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="1" sqref="M41:M43 E24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="2" sqref="A2 J12 E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1023" min="18" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1023" min="18" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,16 +1876,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F69" activeCellId="1" sqref="M41:M43 F69"/>
+      <selection pane="topLeft" activeCell="F69" activeCellId="2" sqref="A2 J12 F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,33 +1974,33 @@
   </sheetPr>
   <dimension ref="1:66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M41" activeCellId="0" sqref="M41:M43"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="J12" activeCellId="1" sqref="A2 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5558,20 +5558,20 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="1" sqref="M41:M43 G38"/>
+      <selection pane="topLeft" activeCell="G38" activeCellId="2" sqref="A2 J12 G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="26" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="26" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="26" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="26" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixing macro linear empty products
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Linear KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="63">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">template_name</t>
   </si>
   <si>
-    <t xml:space="preserve">scene_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
     <t xml:space="preserve">Open Fridge,Fridge Door</t>
   </si>
   <si>
+    <t xml:space="preserve">Off Premise, Hybrid</t>
+  </si>
+  <si>
     <t xml:space="preserve">store</t>
   </si>
   <si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">ZONE1_SKU_ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off Premise, Hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">2,3</t>
@@ -632,33 +629,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI4"/>
+  <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="2" sqref="A2 J12 E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I34" activeCellId="1" sqref="C22 I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1023" min="18" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="47.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.030612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,9 +705,7 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q1" s="0"/>
       <c r="R1" s="0"/>
       <c r="S1" s="0"/>
       <c r="T1" s="0"/>
@@ -1718,54 +1711,50 @@
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
+      <c r="K2" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="L2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>0</v>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1777,40 +1766,37 @@
         <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>21</v>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="L3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>0</v>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1826,34 +1812,31 @@
       </c>
       <c r="D4" s="3"/>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1876,16 +1859,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F69" activeCellId="2" sqref="A2 J12 F69"/>
+      <selection pane="topLeft" activeCell="F69" activeCellId="2" sqref="C22 I34 F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,19 +1890,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,16 +1910,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,16 +1927,16 @@
         <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1974,33 +1957,33 @@
   </sheetPr>
   <dimension ref="1:66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="J12" activeCellId="1" sqref="A2 J12"/>
+      <selection pane="bottomLeft" activeCell="J12" activeCellId="2" sqref="C22 I34 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="46.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="7" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="7" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2015,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>28</v>
@@ -2044,7 +2027,7 @@
         <v>8</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>30</v>
@@ -2053,13 +2036,13 @@
         <v>31</v>
       </c>
       <c r="Q1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="T1" s="0"/>
       <c r="U1" s="0"/>
@@ -3084,32 +3067,32 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L2" s="10" t="n">
         <v>4</v>
       </c>
       <c r="M2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3129,32 +3112,32 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L3" s="10" t="n">
         <v>5</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="73.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3174,34 +3157,34 @@
       <c r="H4" s="11"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L4" s="10" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="R4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3221,7 +3204,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K5" s="10" t="n">
         <v>2</v>
@@ -3230,23 +3213,23 @@
         <v>3</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="53.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3266,32 +3249,32 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="M6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="74.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3311,7 +3294,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K7" s="10" t="n">
         <v>2</v>
@@ -3320,25 +3303,25 @@
         <v>4</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" s="10" t="n">
         <v>1</v>
       </c>
       <c r="O7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="R7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="71.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3358,42 +3341,42 @@
       <c r="H8" s="11"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="M8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10" t="s">
+      <c r="Q8" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="R8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="13" t="n">
         <v>2</v>
@@ -3405,42 +3388,42 @@
       <c r="H9" s="14"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="L9" s="13" t="n">
         <v>5</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N9" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="R9" s="13" t="s">
         <v>23</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="13" t="n">
         <v>2</v>
@@ -3452,7 +3435,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K10" s="13" t="n">
         <v>2</v>
@@ -3461,33 +3444,33 @@
         <v>4</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N10" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="R10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13" t="n">
         <v>2</v>
@@ -3499,42 +3482,42 @@
       <c r="H11" s="14"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="M11" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="R11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="74.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="16" t="n">
         <v>3</v>
@@ -3546,26 +3529,26 @@
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K12" s="16" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>49</v>
-      </c>
       <c r="N12" s="16" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="16" t="s">
         <v>23</v>
@@ -3576,10 +3559,10 @@
     </row>
     <row r="13" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="20" t="n">
         <v>4</v>
@@ -3591,29 +3574,29 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="N13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S13" s="20" t="s">
         <v>24</v>
@@ -3621,10 +3604,10 @@
     </row>
     <row r="14" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="20" t="n">
         <v>4</v>
@@ -3636,29 +3619,29 @@
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="20" t="n">
         <v>4</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P14" s="20"/>
       <c r="Q14" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S14" s="20" t="s">
         <v>24</v>
@@ -3666,10 +3649,10 @@
     </row>
     <row r="15" customFormat="false" ht="30.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="20" t="n">
         <v>4</v>
@@ -3681,29 +3664,29 @@
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N15" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S15" s="20" t="s">
         <v>24</v>
@@ -3711,45 +3694,45 @@
     </row>
     <row r="16" customFormat="false" ht="32.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L16" s="10" t="n">
         <v>4</v>
       </c>
       <c r="M16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N16" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>23</v>
@@ -3760,45 +3743,45 @@
     </row>
     <row r="17" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L17" s="10" t="n">
         <v>5</v>
       </c>
       <c r="M17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N17" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R17" s="10" t="s">
         <v>23</v>
@@ -3809,47 +3792,47 @@
     </row>
     <row r="18" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L18" s="10" t="n">
         <v>5</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N18" s="10" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R18" s="10" t="s">
         <v>23</v>
@@ -3860,26 +3843,26 @@
     </row>
     <row r="19" customFormat="false" ht="63.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K19" s="10" t="n">
         <v>2</v>
@@ -3888,17 +3871,17 @@
         <v>3</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N19" s="10" t="n">
         <v>1</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R19" s="10" t="s">
         <v>23</v>
@@ -3909,45 +3892,45 @@
     </row>
     <row r="20" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="M20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N20" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R20" s="10" t="s">
         <v>23</v>
@@ -3958,26 +3941,26 @@
     </row>
     <row r="21" customFormat="false" ht="67.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K21" s="10" t="n">
         <v>2</v>
@@ -3986,19 +3969,19 @@
         <v>4</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N21" s="10" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R21" s="10" t="s">
         <v>23</v>
@@ -4009,47 +3992,47 @@
     </row>
     <row r="22" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="M22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="Q22" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R22" s="10" t="s">
         <v>23</v>
@@ -4060,47 +4043,47 @@
     </row>
     <row r="23" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="L23" s="13" t="n">
         <v>5</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N23" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q23" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R23" s="13" t="s">
         <v>23</v>
@@ -4111,47 +4094,47 @@
     </row>
     <row r="24" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K24" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="M24" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N24" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q24" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R24" s="13" t="s">
         <v>23</v>
@@ -4162,26 +4145,26 @@
     </row>
     <row r="25" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K25" s="13" t="n">
         <v>2</v>
@@ -4190,19 +4173,19 @@
         <v>4</v>
       </c>
       <c r="M25" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N25" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q25" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R25" s="13" t="s">
         <v>23</v>
@@ -4213,45 +4196,45 @@
     </row>
     <row r="26" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K26" s="16" t="n">
         <v>1</v>
       </c>
       <c r="L26" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="18" t="s">
-        <v>49</v>
-      </c>
       <c r="N26" s="16" t="n">
         <v>1</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P26" s="16"/>
       <c r="Q26" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R26" s="16" t="s">
         <v>23</v>
@@ -4262,26 +4245,26 @@
     </row>
     <row r="27" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K27" s="20" t="n">
         <v>4</v>
@@ -4290,17 +4273,17 @@
         <v>4</v>
       </c>
       <c r="M27" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="N27" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="P27" s="20"/>
       <c r="Q27" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R27" s="20" t="s">
         <v>23</v>
@@ -4311,45 +4294,45 @@
     </row>
     <row r="28" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L28" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M28" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="N28" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="P28" s="20"/>
       <c r="Q28" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R28" s="20" t="s">
         <v>23</v>
@@ -4360,45 +4343,45 @@
     </row>
     <row r="29" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L29" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N29" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P29" s="20"/>
       <c r="Q29" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R29" s="20" t="s">
         <v>23</v>
@@ -4409,26 +4392,26 @@
     </row>
     <row r="30" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K30" s="20" t="n">
         <v>3</v>
@@ -4437,17 +4420,17 @@
         <v>3</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N30" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O30" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P30" s="20"/>
       <c r="Q30" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R30" s="20" t="s">
         <v>23</v>
@@ -4458,45 +4441,45 @@
     </row>
     <row r="31" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M31" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="N31" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O31" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="P31" s="20"/>
       <c r="Q31" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R31" s="20" t="s">
         <v>23</v>
@@ -4507,45 +4490,45 @@
     </row>
     <row r="32" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L32" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M32" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N32" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O32" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P32" s="20"/>
       <c r="Q32" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R32" s="20" t="s">
         <v>23</v>
@@ -4556,45 +4539,45 @@
     </row>
     <row r="33" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L33" s="20" t="n">
         <v>4</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N33" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O33" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P33" s="20"/>
       <c r="Q33" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R33" s="20" t="s">
         <v>23</v>
@@ -4605,33 +4588,33 @@
     </row>
     <row r="34" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L34" s="10" t="n">
         <v>4</v>
@@ -4641,11 +4624,11 @@
         <v>1</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R34" s="10" t="s">
         <v>8</v>
@@ -4656,33 +4639,33 @@
     </row>
     <row r="35" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L35" s="10" t="n">
         <v>5</v>
@@ -4692,11 +4675,11 @@
         <v>1</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R35" s="10" t="s">
         <v>8</v>
@@ -4707,33 +4690,33 @@
     </row>
     <row r="36" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="L36" s="10" t="n">
         <v>5</v>
@@ -4743,13 +4726,13 @@
         <v>1</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R36" s="10" t="s">
         <v>8</v>
@@ -4760,30 +4743,30 @@
     </row>
     <row r="37" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K37" s="10" t="n">
         <v>2</v>
@@ -4796,11 +4779,11 @@
         <v>1</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R37" s="10" t="s">
         <v>8</v>
@@ -4811,36 +4794,36 @@
     </row>
     <row r="38" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="M38" s="10"/>
       <c r="N38" s="10" t="n">
@@ -4849,7 +4832,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
       <c r="Q38" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R38" s="10" t="s">
         <v>8</v>
@@ -4860,30 +4843,30 @@
     </row>
     <row r="39" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K39" s="10" t="n">
         <v>2</v>
@@ -4897,10 +4880,10 @@
       </c>
       <c r="O39" s="10"/>
       <c r="P39" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q39" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R39" s="10" t="s">
         <v>8</v>
@@ -4911,36 +4894,36 @@
     </row>
     <row r="40" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L40" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="L40" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="M40" s="10"/>
       <c r="N40" s="10" t="n">
@@ -4948,10 +4931,10 @@
       </c>
       <c r="O40" s="10"/>
       <c r="P40" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q40" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R40" s="10" t="s">
         <v>8</v>
@@ -4962,33 +4945,33 @@
     </row>
     <row r="41" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="L41" s="13" t="n">
         <v>5</v>
@@ -4998,13 +4981,13 @@
         <v>1</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P41" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q41" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R41" s="13" t="s">
         <v>8</v>
@@ -5015,49 +4998,49 @@
     </row>
     <row r="42" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K42" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L42" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="M42" s="14"/>
       <c r="N42" s="13" t="n">
         <v>1</v>
       </c>
       <c r="O42" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P42" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q42" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R42" s="13" t="s">
         <v>8</v>
@@ -5068,30 +5051,30 @@
     </row>
     <row r="43" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="13"/>
       <c r="G43" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K43" s="13" t="n">
         <v>2</v>
@@ -5104,13 +5087,13 @@
         <v>1</v>
       </c>
       <c r="O43" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P43" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q43" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R43" s="13" t="s">
         <v>8</v>
@@ -5121,47 +5104,47 @@
     </row>
     <row r="44" customFormat="false" ht="83.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F44" s="16"/>
       <c r="G44" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I44" s="16"/>
       <c r="J44" s="16" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K44" s="16" t="n">
         <v>1</v>
       </c>
       <c r="L44" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M44" s="16"/>
       <c r="N44" s="16" t="n">
         <v>1</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P44" s="16"/>
       <c r="Q44" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R44" s="16" t="s">
         <v>8</v>
@@ -5172,33 +5155,33 @@
     </row>
     <row r="45" customFormat="false" ht="46.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L45" s="20" t="n">
         <v>4</v>
@@ -5208,11 +5191,11 @@
         <v>1</v>
       </c>
       <c r="O45" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P45" s="20"/>
       <c r="Q45" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R45" s="20" t="s">
         <v>8</v>
@@ -5223,47 +5206,47 @@
     </row>
     <row r="46" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L46" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M46" s="20"/>
       <c r="N46" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O46" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P46" s="20"/>
       <c r="Q46" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R46" s="20" t="s">
         <v>8</v>
@@ -5274,47 +5257,47 @@
     </row>
     <row r="47" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L47" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M47" s="20"/>
       <c r="N47" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O47" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P47" s="20"/>
       <c r="Q47" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R47" s="20" t="s">
         <v>8</v>
@@ -5325,30 +5308,30 @@
     </row>
     <row r="48" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K48" s="20" t="n">
         <v>4</v>
@@ -5361,11 +5344,11 @@
         <v>1</v>
       </c>
       <c r="O48" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P48" s="20"/>
       <c r="Q48" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R48" s="20" t="s">
         <v>8</v>
@@ -5376,33 +5359,33 @@
     </row>
     <row r="49" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L49" s="20" t="n">
         <v>5</v>
@@ -5412,11 +5395,11 @@
         <v>1</v>
       </c>
       <c r="O49" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P49" s="20"/>
       <c r="Q49" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R49" s="20" t="s">
         <v>8</v>
@@ -5427,33 +5410,33 @@
     </row>
     <row r="50" customFormat="false" ht="53.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I50" s="20"/>
       <c r="J50" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L50" s="20" t="n">
         <v>5</v>
@@ -5463,11 +5446,11 @@
         <v>1</v>
       </c>
       <c r="O50" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P50" s="20"/>
       <c r="Q50" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R50" s="20" t="s">
         <v>8</v>
@@ -5478,30 +5461,30 @@
     </row>
     <row r="51" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="20" t="n">
         <v>4</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I51" s="20"/>
       <c r="J51" s="20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K51" s="20" t="n">
         <v>3</v>
@@ -5514,11 +5497,11 @@
         <v>1</v>
       </c>
       <c r="O51" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P51" s="20"/>
       <c r="Q51" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R51" s="20" t="s">
         <v>8</v>
@@ -5558,20 +5541,20 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="2" sqref="A2 J12 G38"/>
+      <selection pane="topLeft" activeCell="G38" activeCellId="2" sqref="C22 I34 G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="26" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="26" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="26" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="26" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5596,14 +5579,14 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="30"/>
       <c r="G2" s="28"/>
@@ -5612,14 +5595,14 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="30"/>
       <c r="G3" s="28"/>
@@ -5628,14 +5611,14 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="30"/>
       <c r="G4" s="28"/>
@@ -5644,14 +5627,14 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="30"/>
       <c r="G5" s="28"/>
@@ -5660,54 +5643,54 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="33"/>
       <c r="G6" s="34"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="33"/>
     </row>

</xml_diff>

<commit_message>
adding more scene types to macro
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="63">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -86,6 +86,90 @@
   </si>
   <si>
     <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fridge Door, Open Fridge, Ambient Shelf, Open Impulse Fridge, TWE Standalone Fridge, TWE Impulse Fridge Door, TWE Open Impulse Fridge, Impulse Fridge Door, Standalone Fridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off Premise, Hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf_policy_from_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_of_shelves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irrelevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_include_policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMON_ZONE1_SKU_ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Fridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_fk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standalone Fridge,
+TWE Standalone Fridge,
+Fridge Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excl(1,N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Impulse Fridge,
+TWE Open Impulse Fridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excl (1,N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMON_ZONE2_SKU_ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only(1,N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMON_ZONE3_SKU_ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,4,5,6,7</t>
   </si>
   <si>
     <t xml:space="preserve">Open Fridge,
@@ -94,87 +178,6 @@
 Standalone Fridge,
 TWE Open Impulse Fridge,
 TWE Standalone Fridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off Premise, Hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelf_policy_from_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number_of_shelves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">irrelevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_include_policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMON_ZONE1_SKU_ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open Fridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standalone Fridge,
-TWE Standalone Fridge,
-Fridge Door</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excl(1,N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open Impulse Fridge,
-TWE Open Impulse Fridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excl (1,N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMON_ZONE2_SKU_ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only(1,N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMON_ZONE3_SKU_ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,4,5,6,7</t>
   </si>
   <si>
     <t xml:space="preserve">SIMON_ZONE4_SKU_ALL</t>
@@ -644,28 +647,14 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="47.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2908163265306"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.9234693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1022" min="17" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1022" min="1" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="28.2142857142857"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,7 +707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="71.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="161.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -764,7 +753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="71.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="161.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -806,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="69.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -868,17 +857,17 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="47.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,32 +956,32 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="V8" activeCellId="0" sqref="V8"/>
+      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="46.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="16.0561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="14.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.9387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="19.6479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.6071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="19.6479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="16.0561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.18877551020408"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="10.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="22.4285714285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="16.0561224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="46.3826530612245"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1531,7 @@
         <v>47</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="N12" s="23" t="n">
         <v>1</v>
@@ -1563,10 +1552,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="27" t="n">
         <v>4</v>
@@ -1581,7 +1570,7 @@
         <v>22</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L13" s="27" t="s">
         <v>42</v>
@@ -1608,10 +1597,10 @@
     </row>
     <row r="14" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="27" t="n">
         <v>4</v>
@@ -1626,7 +1615,7 @@
         <v>22</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L14" s="27" t="n">
         <v>4</v>
@@ -1653,10 +1642,10 @@
     </row>
     <row r="15" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="27" t="n">
         <v>4</v>
@@ -1671,7 +1660,7 @@
         <v>22</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L15" s="27" t="s">
         <v>42</v>
@@ -1698,10 +1687,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="17" t="n">
         <v>1</v>
@@ -1747,10 +1736,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="17" t="n">
         <v>1</v>
@@ -1796,10 +1785,10 @@
     </row>
     <row r="18" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="17" t="n">
         <v>1</v>
@@ -1847,10 +1836,10 @@
     </row>
     <row r="19" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="17" t="n">
         <v>1</v>
@@ -1896,10 +1885,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" s="17" t="n">
         <v>1</v>
@@ -1945,10 +1934,10 @@
     </row>
     <row r="21" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>1</v>
@@ -1996,10 +1985,10 @@
     </row>
     <row r="22" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>1</v>
@@ -2047,10 +2036,10 @@
     </row>
     <row r="23" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="20" t="n">
         <v>2</v>
@@ -2098,10 +2087,10 @@
     </row>
     <row r="24" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="20" t="n">
         <v>2</v>
@@ -2149,10 +2138,10 @@
     </row>
     <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="20" t="n">
         <v>2</v>
@@ -2200,10 +2189,10 @@
     </row>
     <row r="26" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>3</v>
@@ -2228,7 +2217,7 @@
         <v>47</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="N26" s="23" t="n">
         <v>1</v>
@@ -2249,10 +2238,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="27" t="n">
         <v>4</v>
@@ -2298,10 +2287,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" s="27" t="n">
         <v>4</v>
@@ -2320,7 +2309,7 @@
         <v>22</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" s="27" t="n">
         <v>5</v>
@@ -2347,10 +2336,10 @@
     </row>
     <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="27" t="n">
         <v>4</v>
@@ -2369,7 +2358,7 @@
         <v>22</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L29" s="27" t="n">
         <v>5</v>
@@ -2396,10 +2385,10 @@
     </row>
     <row r="30" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="27" t="n">
         <v>4</v>
@@ -2424,7 +2413,7 @@
         <v>3</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N30" s="27" t="n">
         <v>1</v>
@@ -2445,10 +2434,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C31" s="27" t="n">
         <v>4</v>
@@ -2467,7 +2456,7 @@
         <v>22</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L31" s="27" t="s">
         <v>42</v>
@@ -2494,10 +2483,10 @@
     </row>
     <row r="32" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C32" s="27" t="n">
         <v>4</v>
@@ -2516,7 +2505,7 @@
         <v>22</v>
       </c>
       <c r="K32" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L32" s="27" t="s">
         <v>42</v>
@@ -2543,10 +2532,10 @@
     </row>
     <row r="33" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33" s="27" t="n">
         <v>4</v>
@@ -2565,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="K33" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L33" s="27" t="n">
         <v>4</v>
@@ -2592,10 +2581,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C34" s="17" t="n">
         <v>1</v>
@@ -2643,10 +2632,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" s="17" t="n">
         <v>1</v>
@@ -2694,10 +2683,10 @@
     </row>
     <row r="36" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" s="17" t="n">
         <v>1</v>
@@ -2747,10 +2736,10 @@
     </row>
     <row r="37" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C37" s="17" t="n">
         <v>1</v>
@@ -2766,7 +2755,7 @@
         <v>19</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="17" t="s">
@@ -2798,10 +2787,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C38" s="17" t="n">
         <v>1</v>
@@ -2847,10 +2836,10 @@
     </row>
     <row r="39" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>1</v>
@@ -2898,10 +2887,10 @@
     </row>
     <row r="40" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>1</v>
@@ -2949,10 +2938,10 @@
     </row>
     <row r="41" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="20" t="n">
         <v>2</v>
@@ -3002,10 +2991,10 @@
     </row>
     <row r="42" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="20" t="n">
         <v>2</v>
@@ -3055,10 +3044,10 @@
     </row>
     <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C43" s="20" t="n">
         <v>2</v>
@@ -3108,10 +3097,10 @@
     </row>
     <row r="44" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C44" s="23" t="n">
         <v>3</v>
@@ -3127,7 +3116,7 @@
         <v>19</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23" t="s">
@@ -3159,10 +3148,10 @@
     </row>
     <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C45" s="27" t="n">
         <v>4</v>
@@ -3185,7 +3174,7 @@
         <v>22</v>
       </c>
       <c r="K45" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L45" s="27" t="n">
         <v>4</v>
@@ -3210,10 +3199,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C46" s="27" t="n">
         <v>4</v>
@@ -3236,7 +3225,7 @@
         <v>22</v>
       </c>
       <c r="K46" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L46" s="27" t="s">
         <v>42</v>
@@ -3261,10 +3250,10 @@
     </row>
     <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C47" s="27" t="n">
         <v>4</v>
@@ -3287,7 +3276,7 @@
         <v>22</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L47" s="27" t="s">
         <v>42</v>
@@ -3312,10 +3301,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C48" s="27" t="n">
         <v>4</v>
@@ -3363,10 +3352,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C49" s="27" t="n">
         <v>4</v>
@@ -3389,7 +3378,7 @@
         <v>22</v>
       </c>
       <c r="K49" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L49" s="27" t="n">
         <v>5</v>
@@ -3414,10 +3403,10 @@
     </row>
     <row r="50" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50" s="27" t="n">
         <v>4</v>
@@ -3440,7 +3429,7 @@
         <v>22</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L50" s="27" t="n">
         <v>5</v>
@@ -3465,10 +3454,10 @@
     </row>
     <row r="51" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C51" s="27" t="n">
         <v>4</v>
@@ -3484,7 +3473,7 @@
         <v>19</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
@@ -3532,21 +3521,21 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3571,7 +3560,7 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>17</v>
@@ -3587,7 +3576,7 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>17</v>
@@ -3603,7 +3592,7 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>17</v>
@@ -3619,7 +3608,7 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>17</v>
@@ -3635,7 +3624,7 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>17</v>
@@ -3649,7 +3638,7 @@
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>17</v>
@@ -3662,7 +3651,7 @@
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -3675,7 +3664,7 @@
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
added parent relation for macro linear
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -23,7 +23,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="64">
+  <si>
+    <t xml:space="preserve">kpi_parent_name</t>
+  </si>
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -412,14 +415,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -428,7 +431,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,7 +443,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,23 +648,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1022" min="1" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="2" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.7448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="52.7448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="40.4183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="45.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.8061224489796"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -706,13 +715,14 @@
       <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="161.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="113.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>17</v>
@@ -720,123 +730,130 @@
       <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="M2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="O2" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="161.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>25</v>
+      <c r="Q2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="121.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="6" t="n">
+      <c r="K3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="M3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="O3" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="Q3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="9" t="n">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="9" t="n">
-        <v>1</v>
-      </c>
       <c r="M4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>8</v>
+      <c r="O4" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -857,85 +874,85 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="46.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="46.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -956,99 +973,100 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="45.4897959183674"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="46.3826530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>1</v>
@@ -1060,40 +1078,40 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L2" s="17" t="n">
         <v>4</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N2" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>1</v>
@@ -1105,40 +1123,40 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L3" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N3" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P3" s="17"/>
       <c r="Q3" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>1</v>
@@ -1150,42 +1168,42 @@
       <c r="H4" s="18"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L4" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="N4" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>1</v>
@@ -1197,7 +1215,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" s="17" t="n">
         <v>2</v>
@@ -1206,31 +1224,31 @@
         <v>3</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P5" s="17"/>
       <c r="Q5" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>1</v>
@@ -1242,40 +1260,40 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N6" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P6" s="17"/>
       <c r="Q6" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S6" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>1</v>
@@ -1287,7 +1305,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K7" s="17" t="n">
         <v>2</v>
@@ -1296,33 +1314,33 @@
         <v>4</v>
       </c>
       <c r="M7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="N7" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>1</v>
@@ -1334,42 +1352,42 @@
       <c r="H8" s="18"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="N8" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="20" t="n">
         <v>2</v>
@@ -1381,42 +1399,42 @@
       <c r="H9" s="21"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L9" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M9" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="N9" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="20" t="n">
         <v>2</v>
@@ -1428,7 +1446,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K10" s="20" t="n">
         <v>2</v>
@@ -1437,33 +1455,33 @@
         <v>4</v>
       </c>
       <c r="M10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="N10" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="20" t="n">
         <v>2</v>
@@ -1475,42 +1493,42 @@
       <c r="H11" s="21"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M11" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S11" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="N11" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="23" t="n">
         <v>3</v>
@@ -1522,40 +1540,40 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P12" s="23"/>
       <c r="Q12" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S12" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="27" t="n">
         <v>4</v>
@@ -1567,40 +1585,40 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N13" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P13" s="27"/>
       <c r="Q13" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S13" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="27" t="n">
         <v>4</v>
@@ -1612,40 +1630,40 @@
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L14" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M14" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N14" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P14" s="27"/>
       <c r="Q14" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S14" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="27" t="n">
         <v>4</v>
@@ -1657,205 +1675,205 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L15" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M15" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N15" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P15" s="27"/>
       <c r="Q15" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R15" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L16" s="17" t="n">
         <v>4</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N16" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P16" s="17"/>
       <c r="Q16" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S16" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L17" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N17" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P17" s="17"/>
       <c r="Q17" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S17" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L18" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N18" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q18" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S18" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K19" s="17" t="n">
         <v>2</v>
@@ -1864,96 +1882,96 @@
         <v>3</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N19" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P20" s="17"/>
       <c r="Q20" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K21" s="17" t="n">
         <v>2</v>
@@ -1962,202 +1980,202 @@
         <v>4</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N21" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q21" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N22" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q22" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S22" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L23" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N23" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O23" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q23" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R23" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S23" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L24" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N24" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q24" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S24" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K25" s="20" t="n">
         <v>2</v>
@@ -2166,98 +2184,98 @@
         <v>4</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N25" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q25" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R25" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S25" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>3</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K26" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N26" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P26" s="23"/>
       <c r="Q26" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R26" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S26" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
       <c r="J27" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K27" s="27" t="n">
         <v>4</v>
@@ -2266,145 +2284,145 @@
         <v>4</v>
       </c>
       <c r="M27" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N27" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O27" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P27" s="27"/>
       <c r="Q27" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R27" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S27" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
       <c r="J28" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L28" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M28" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N28" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O28" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P28" s="27"/>
       <c r="Q28" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R28" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S28" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L29" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N29" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O29" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P29" s="27"/>
       <c r="Q29" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R29" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S29" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K30" s="27" t="n">
         <v>3</v>
@@ -2413,201 +2431,201 @@
         <v>3</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N30" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O30" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P30" s="27"/>
       <c r="Q30" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R30" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S30" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L31" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M31" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N31" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P31" s="27"/>
       <c r="Q31" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S31" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K32" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L32" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M32" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N32" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P32" s="27"/>
       <c r="Q32" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S32" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K33" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L33" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N33" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P33" s="27"/>
       <c r="Q33" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S33" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L34" s="17" t="n">
         <v>4</v>
@@ -2617,48 +2635,48 @@
         <v>1</v>
       </c>
       <c r="O34" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P34" s="17"/>
       <c r="Q34" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S34" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I35" s="17"/>
       <c r="J35" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L35" s="17" t="n">
         <v>5</v>
@@ -2668,48 +2686,48 @@
         <v>1</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P35" s="17"/>
       <c r="Q35" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R35" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S35" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C36" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L36" s="17" t="n">
         <v>5</v>
@@ -2719,47 +2737,47 @@
         <v>1</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P36" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q36" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S36" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K37" s="17" t="n">
         <v>2</v>
@@ -2772,51 +2790,51 @@
         <v>1</v>
       </c>
       <c r="O37" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P37" s="17"/>
       <c r="Q37" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S37" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C38" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17" t="n">
@@ -2825,41 +2843,41 @@
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S38" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K39" s="17" t="n">
         <v>2</v>
@@ -2873,50 +2891,50 @@
       </c>
       <c r="O39" s="17"/>
       <c r="P39" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q39" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S39" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M40" s="17"/>
       <c r="N40" s="17" t="n">
@@ -2924,47 +2942,47 @@
       </c>
       <c r="O40" s="17"/>
       <c r="P40" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q40" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S40" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K41" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L41" s="20" t="n">
         <v>5</v>
@@ -2974,100 +2992,100 @@
         <v>1</v>
       </c>
       <c r="O41" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q41" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R41" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S41" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F42" s="20"/>
       <c r="G42" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L42" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M42" s="21"/>
       <c r="N42" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O42" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q42" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R42" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S42" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C43" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K43" s="20" t="n">
         <v>2</v>
@@ -3080,101 +3098,101 @@
         <v>1</v>
       </c>
       <c r="O43" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q43" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R43" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S43" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C44" s="23" t="n">
         <v>3</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F44" s="23"/>
       <c r="G44" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K44" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L44" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M44" s="23"/>
       <c r="N44" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O44" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P44" s="23"/>
       <c r="Q44" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R44" s="23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S44" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C45" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F45" s="27"/>
       <c r="G45" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H45" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I45" s="27"/>
       <c r="J45" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K45" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L45" s="27" t="n">
         <v>4</v>
@@ -3184,147 +3202,147 @@
         <v>1</v>
       </c>
       <c r="O45" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P45" s="27"/>
       <c r="Q45" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R45" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S45" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F46" s="27"/>
       <c r="G46" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H46" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I46" s="27"/>
       <c r="J46" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K46" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L46" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M46" s="27"/>
       <c r="N46" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O46" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P46" s="27"/>
       <c r="Q46" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R46" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S46" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C47" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I47" s="27"/>
       <c r="J47" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L47" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M47" s="27"/>
       <c r="N47" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O47" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P47" s="27"/>
       <c r="Q47" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R47" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S47" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C48" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H48" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I48" s="27"/>
       <c r="J48" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K48" s="27" t="n">
         <v>4</v>
@@ -3337,48 +3355,48 @@
         <v>1</v>
       </c>
       <c r="O48" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P48" s="27"/>
       <c r="Q48" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R48" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S48" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C49" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K49" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L49" s="27" t="n">
         <v>5</v>
@@ -3388,48 +3406,48 @@
         <v>1</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P49" s="27"/>
       <c r="Q49" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R49" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S49" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C50" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H50" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L50" s="27" t="n">
         <v>5</v>
@@ -3439,45 +3457,45 @@
         <v>1</v>
       </c>
       <c r="O50" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P50" s="27"/>
       <c r="Q50" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R50" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S50" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K51" s="27" t="n">
         <v>3</v>
@@ -3490,17 +3508,17 @@
         <v>1</v>
       </c>
       <c r="O51" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P51" s="27"/>
       <c r="Q51" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R51" s="27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S51" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3521,38 +3539,38 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
@@ -3560,14 +3578,14 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="9"/>
       <c r="G2" s="34"/>
@@ -3576,14 +3594,14 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="9"/>
       <c r="G3" s="34"/>
@@ -3592,14 +3610,14 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9"/>
       <c r="G4" s="34"/>
@@ -3608,14 +3626,14 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="9"/>
       <c r="G5" s="34"/>
@@ -3624,56 +3642,56 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="E6" s="5"/>
       <c r="G6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
facing zero ignored in macro linear
</commit_message>
<xml_diff>
--- a/Projects/TWEAU/Data/Template.xlsx
+++ b/Projects/TWEAU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Linear KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="64">
   <si>
     <t xml:space="preserve">kpi_parent_name</t>
   </si>
@@ -184,24 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">SIMON_ZONE4_SKU_ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZONE1_OWN_MANUFACTURER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZONE2_OWN_MANUFACTURER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZONE3_OWN_MANUFACTURER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZONE4_OWN_MANUFACTURER</t>
   </si>
   <si>
     <t xml:space="preserve">4,5</t>
@@ -228,6 +210,24 @@
       </rPr>
       <t xml:space="preserve">TWE Open Impulse Fridge</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">5,6,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZONE1_OWN_MANUFACTURER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZONE2_OWN_MANUFACTURER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZONE3_OWN_MANUFACTURER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZONE4_OWN_MANUFACTURER</t>
   </si>
   <si>
     <t xml:space="preserve">ZONE1_OWN_MANUFACTURER_PER_SCENE_TYPE</t>
@@ -309,18 +309,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Ariel"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -527,7 +527,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,7 +535,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -650,20 +650,20 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.7448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="52.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="40.4183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="45.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="52.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.5408163265306"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,11 +880,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,35 +971,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="44.8163265306122"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,11 +1587,11 @@
       <c r="J13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="27" t="s">
-        <v>43</v>
+      <c r="K13" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="L13" s="27" t="n">
+        <v>4</v>
       </c>
       <c r="M13" s="27" t="s">
         <v>35</v>
@@ -1607,13 +1607,13 @@
         <v>37</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="S13" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
         <v>50</v>
       </c>
@@ -1633,13 +1633,13 @@
         <v>23</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="M14" s="28" t="s">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="N14" s="27" t="n">
         <v>1</v>
@@ -1652,13 +1652,13 @@
         <v>37</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="S14" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
         <v>50</v>
       </c>
@@ -1680,8 +1680,8 @@
       <c r="K15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="27" t="s">
-        <v>43</v>
+      <c r="L15" s="27" t="n">
+        <v>5</v>
       </c>
       <c r="M15" s="28" t="s">
         <v>39</v>
@@ -1697,216 +1697,190 @@
         <v>37</v>
       </c>
       <c r="R15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="21.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="S15" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+      <c r="R16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="L17" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17" s="27"/>
+    </row>
+    <row r="18" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="27"/>
+    </row>
+    <row r="19" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="R16" s="17" t="s">
+      <c r="L19" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="S16" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="R17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S17" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P18" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q18" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S18" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="L19" s="17" t="n">
-        <v>3</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="N19" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O19" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S19" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="S19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C20" s="17" t="n">
         <v>1</v>
@@ -1925,10 +1899,10 @@
         <v>23</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="L20" s="17" t="n">
+        <v>4</v>
       </c>
       <c r="M20" s="17" t="s">
         <v>35</v>
@@ -1950,12 +1924,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>1</v>
@@ -1973,14 +1947,14 @@
       <c r="J21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="17" t="n">
-        <v>2</v>
+      <c r="K21" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="L21" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="M21" s="18" t="s">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="N21" s="17" t="n">
         <v>1</v>
@@ -1988,9 +1962,7 @@
       <c r="O21" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P21" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="P21" s="17"/>
       <c r="Q21" s="30" t="s">
         <v>18</v>
       </c>
@@ -2003,10 +1975,10 @@
     </row>
     <row r="22" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>1</v>
@@ -2025,10 +1997,10 @@
         <v>23</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="L22" s="17" t="n">
+        <v>5</v>
       </c>
       <c r="M22" s="18" t="s">
         <v>39</v>
@@ -2052,410 +2024,414 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="20" t="n">
+    <row r="23" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="20" t="s">
+      <c r="L23" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S23" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S24" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="L25" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q25" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S25" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S26" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="L23" s="20" t="n">
+      <c r="L27" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="M23" s="21" t="s">
+      <c r="M27" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N23" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O23" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P23" s="20" t="s">
+      <c r="N27" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q23" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="R23" s="20" t="s">
+      <c r="Q27" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="S23" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="20" t="n">
+      <c r="S27" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="20" t="s">
+      <c r="D28" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="20" t="s">
+      <c r="L28" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="M28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N24" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O24" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P24" s="20" t="s">
+      <c r="N28" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P28" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q24" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="R24" s="20" t="s">
+      <c r="Q28" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="R28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="S24" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="20" t="n">
+      <c r="S28" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="20" t="n">
+      <c r="D29" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="L25" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="M25" s="21" t="s">
+      <c r="L29" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="M29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P25" s="20" t="s">
+      <c r="N29" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q25" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="R25" s="20" t="s">
+      <c r="Q29" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="R29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="S25" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="23" t="n">
+      <c r="S29" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K26" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="L26" s="23" t="s">
+      <c r="D30" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="25" t="s">
+      <c r="M30" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="N26" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="R26" s="23" t="s">
+      <c r="N30" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="R30" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="S26" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="L27" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="M27" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O27" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R27" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S27" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="L28" s="27" t="n">
-        <v>5</v>
-      </c>
-      <c r="M28" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R28" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S28" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K29" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="L29" s="27" t="n">
-        <v>5</v>
-      </c>
-      <c r="M29" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="N29" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O29" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R29" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S29" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="L30" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="N30" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O30" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R30" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S30" s="27" t="s">
+      <c r="S30" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C31" s="27" t="n">
         <v>4</v>
@@ -2473,11 +2449,11 @@
       <c r="J31" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="27" t="s">
-        <v>43</v>
+      <c r="K31" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="L31" s="27" t="n">
+        <v>4</v>
       </c>
       <c r="M31" s="27" t="s">
         <v>35</v>
@@ -2499,12 +2475,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C32" s="27" t="n">
         <v>4</v>
@@ -2525,11 +2501,11 @@
       <c r="K32" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="L32" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="M32" s="28" t="s">
-        <v>39</v>
+      <c r="L32" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="N32" s="27" t="n">
         <v>1</v>
@@ -2550,10 +2526,10 @@
     </row>
     <row r="33" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33" s="27" t="n">
         <v>4</v>
@@ -2572,10 +2548,10 @@
         <v>23</v>
       </c>
       <c r="K33" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L33" s="27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M33" s="28" t="s">
         <v>39</v>
@@ -2597,209 +2573,199 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="17" t="s">
+    <row r="34" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="L34" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="M34" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R34" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S34" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L34" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="R34" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="S34" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L35" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="R35" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="S35" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="18" t="s">
+      <c r="N35" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R35" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S35" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L36" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="R36" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="S36" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="L37" s="17" t="n">
-        <v>3</v>
-      </c>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O37" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="R37" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="S37" s="17" t="s">
+      <c r="N36" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R36" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S36" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="L37" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="M37" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N37" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S37" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2831,16 +2797,18 @@
         <v>23</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="L38" s="17" t="n">
+        <v>4</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O38" s="17"/>
+      <c r="O38" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="P38" s="17"/>
       <c r="Q38" s="17" t="s">
         <v>18</v>
@@ -2852,7 +2820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
         <v>59</v>
       </c>
@@ -2872,27 +2840,27 @@
       <c r="G39" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="18" t="s">
-        <v>39</v>
+      <c r="H39" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="17" t="n">
-        <v>2</v>
+      <c r="K39" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="L39" s="17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="O39" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P39" s="17"/>
       <c r="Q39" s="17" t="s">
         <v>18</v>
       </c>
@@ -2931,16 +2899,18 @@
         <v>23</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L40" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="L40" s="17" t="n">
+        <v>5</v>
       </c>
       <c r="M40" s="17"/>
       <c r="N40" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O40" s="17"/>
+      <c r="O40" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="P40" s="17" t="s">
         <v>44</v>
       </c>
@@ -2955,420 +2925,418 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="L41" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R41" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="S41" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="S42" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R43" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="S43" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R44" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="S44" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B45" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="20" t="n">
+      <c r="C45" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="21" t="s">
+      <c r="D45" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K41" s="20" t="s">
+      <c r="I45" s="20"/>
+      <c r="J45" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="L41" s="20" t="n">
+      <c r="L45" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="M41" s="21"/>
-      <c r="N41" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O41" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P41" s="20" t="s">
+      <c r="M45" s="21"/>
+      <c r="N45" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O45" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P45" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="R41" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="S41" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19" t="s">
+      <c r="Q45" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="R45" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S45" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="20" t="n">
+      <c r="C46" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="21" t="s">
+      <c r="D46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K42" s="20" t="s">
+      <c r="I46" s="20"/>
+      <c r="J46" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="L42" s="20" t="s">
+      <c r="L46" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="M42" s="21"/>
-      <c r="N42" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O42" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P42" s="20" t="s">
+      <c r="M46" s="21"/>
+      <c r="N46" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P46" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q42" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="R42" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="S42" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19" t="s">
+      <c r="Q46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="R46" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S46" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B47" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="20" t="n">
+      <c r="C47" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43" s="21" t="s">
+      <c r="D47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="20" t="n">
+      <c r="I47" s="20"/>
+      <c r="J47" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="L43" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="M43" s="21"/>
-      <c r="N43" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O43" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P43" s="20" t="s">
+      <c r="L47" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="M47" s="21"/>
+      <c r="N47" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="P47" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Q43" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="R43" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="S43" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
+      <c r="Q47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="R47" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S47" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B48" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="23" t="n">
+      <c r="C48" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="D44" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="25" t="s">
+      <c r="D48" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="L44" s="23" t="s">
+      <c r="I48" s="23"/>
+      <c r="J48" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L48" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O44" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="R44" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="S44" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K45" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="L45" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O45" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R45" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S45" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K46" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="L46" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O46" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R46" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S46" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H47" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K47" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="L47" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O47" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P47" s="27"/>
-      <c r="Q47" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R47" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S47" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K48" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="L48" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O48" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="R48" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S48" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M48" s="23"/>
+      <c r="N48" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="P48" s="23"/>
+      <c r="Q48" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="R48" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S48" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="s">
         <v>63</v>
       </c>
@@ -3388,18 +3356,18 @@
       <c r="G49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H49" s="27" t="s">
-        <v>35</v>
+      <c r="H49" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K49" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L49" s="27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M49" s="27"/>
       <c r="N49" s="27" t="n">
@@ -3419,7 +3387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
         <v>63</v>
       </c>
@@ -3439,18 +3407,18 @@
       <c r="G50" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H50" s="28" t="s">
-        <v>39</v>
+      <c r="H50" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="L50" s="27" t="n">
-        <v>5</v>
+        <v>53</v>
+      </c>
+      <c r="L50" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="M50" s="27"/>
       <c r="N50" s="27" t="n">
@@ -3491,17 +3459,17 @@
         <v>20</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K51" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="L51" s="27" t="n">
-        <v>3</v>
+      <c r="K51" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="L51" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="M51" s="27"/>
       <c r="N51" s="27" t="n">
@@ -3518,6 +3486,210 @@
         <v>9</v>
       </c>
       <c r="S51" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K52" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="L52" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="M52" s="27"/>
+      <c r="N52" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P52" s="27"/>
+      <c r="Q52" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R52" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S52" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L53" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="M53" s="27"/>
+      <c r="N53" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P53" s="27"/>
+      <c r="Q53" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R53" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S53" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R54" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S54" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K55" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="L55" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="M55" s="27"/>
+      <c r="N55" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O55" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="P55" s="27"/>
+      <c r="Q55" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R55" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S55" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3545,15 +3717,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3578,7 +3750,7 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>18</v>
@@ -3610,7 +3782,7 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>18</v>
@@ -3642,7 +3814,7 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>18</v>
@@ -3669,7 +3841,7 @@
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>

</xml_diff>